<commit_message>
gpio test result update
</commit_message>
<xml_diff>
--- a/document/gpio_test_result.xlsx
+++ b/document/gpio_test_result.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>GPA0</t>
   </si>
@@ -165,6 +165,10 @@
   </si>
   <si>
     <t>0: CPU_GPIO39, 1~3:CPU_GPIO57~59, 4~7 : CPU_AIN3~0_ANALOG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SYSLABII baseboard</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -501,7 +505,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -509,7 +513,7 @@
     <col min="6" max="6" width="32.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -522,8 +526,11 @@
       <c r="D1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -537,7 +544,7 @@
         <v>22222222</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -551,7 +558,7 @@
         <v>2222</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -565,7 +572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -579,7 +586,7 @@
         <v>44444</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -593,7 +600,7 @@
         <v>22022</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -607,7 +614,7 @@
         <v>22222222</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -621,7 +628,7 @@
         <v>222222</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -635,7 +642,7 @@
         <v>22222200</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -649,7 +656,7 @@
         <v>22222222</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -663,7 +670,7 @@
         <v>22222222</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -677,7 +684,7 @@
         <v>2222</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -691,7 +698,7 @@
         <v>222222</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -705,7 +712,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -719,7 +726,7 @@
         <v>2222222</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>

</xml_diff>